<commit_message>
Dosyaya döküm adı eklendi
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\can.sarihan\Documents\UiPath\RPA_Cogi_Döküm_REF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FAE8C9-75D4-4636-B90F-2880F9B0516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631AF10E-4594-440E-BFCA-0A7B70F5736E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -803,7 +803,7 @@
         <v>53</v>
       </c>
       <c r="B15" s="10">
-        <v>3002</v>
+        <v>3001</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>58</v>

</xml_diff>